<commit_message>
3 RRIDs added for OMAP-17
blank RRIDs for discontinued antibodies were registered June 5, 2024; these have been added to OMAP
</commit_message>
<xml_diff>
--- a/digital-objects/omap/17-thymus-ibex/v1.0/raw/omap-17-thymus-ibex.xlsx
+++ b/digital-objects/omap/17-thymus-ibex/v1.0/raw/omap-17-thymus-ibex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellenmq/Documents/GitHub/hra-kg/digital-objects/omap/17-thymus-ibex/v1.0/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4272DE93-7618-8747-A3FD-1FE12B35F116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB4B868-5303-A347-8CDE-DE5FBA2FFCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="4500" windowWidth="34560" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OMAP-17-Thymus-with IBEX" sheetId="1" r:id="rId1"/>
@@ -5185,13 +5185,13 @@
     <t>used to detect AT2R, see above</t>
   </si>
   <si>
-    <t>DISCONTINUED:00001</t>
-  </si>
-  <si>
-    <t>DISCONTINUED:00002</t>
-  </si>
-  <si>
-    <t>DISCONTINUED:00003</t>
+    <t>AB_3101791</t>
+  </si>
+  <si>
+    <t>AB_3101792</t>
+  </si>
+  <si>
+    <t>AB_2736945</t>
   </si>
 </sst>
 </file>
@@ -5902,7 +5902,7 @@
   <dimension ref="A1:AR995"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -8894,7 +8894,7 @@
         <v>108</v>
       </c>
       <c r="P37" s="30" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="Q37" s="2" t="s">
         <v>58</v>
@@ -8980,7 +8980,7 @@
         <v>75</v>
       </c>
       <c r="P38" s="30" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>58</v>
@@ -9542,7 +9542,7 @@
         <v>86</v>
       </c>
       <c r="P44" s="30" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>58</v>

</xml_diff>